<commit_message>
dropping inst after write
</commit_message>
<xml_diff>
--- a/HW3/autogen/CUSignals.xlsx
+++ b/HW3/autogen/CUSignals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garre\Desktop\EE 188\HW3\autogen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2660E3C2-B2A8-44EB-A889-82F4B57EF3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D51593-09B9-4ADF-AE7D-341757150D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -2295,7 +2295,7 @@
       </c>
       <c r="L3" s="8">
         <f>PAU!D3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="8" t="str">
         <f>PAU!E3</f>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="L4" s="8">
         <f>PAU!D4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="8" t="str">
         <f>PAU!E4</f>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="L6" s="8">
         <f>PAU!D6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" s="8" t="str">
         <f>PAU!E6</f>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="L7" s="8">
         <f>PAU!D7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="8" t="str">
         <f>PAU!E7</f>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="L8" s="8">
         <f>PAU!D8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="8" t="str">
         <f>PAU!E8</f>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="L9" s="8">
         <f>PAU!D9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="8" t="str">
         <f>PAU!E9</f>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="L10" s="8">
         <f>PAU!D10</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="8" t="str">
         <f>PAU!E10</f>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="L11" s="8">
         <f>PAU!D11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="8" t="str">
         <f>PAU!E11</f>
@@ -3933,7 +3933,7 @@
       </c>
       <c r="L12" s="8">
         <f>PAU!D12</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" s="8" t="str">
         <f>PAU!E12</f>
@@ -4115,7 +4115,7 @@
       </c>
       <c r="L13" s="8">
         <f>PAU!D13</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="8" t="str">
         <f>PAU!E13</f>
@@ -4297,7 +4297,7 @@
       </c>
       <c r="L14" s="8">
         <f>PAU!D14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="8" t="str">
         <f>PAU!E14</f>
@@ -4479,7 +4479,7 @@
       </c>
       <c r="L15" s="8">
         <f>PAU!D15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15" s="8" t="str">
         <f>PAU!E15</f>
@@ -4661,7 +4661,7 @@
       </c>
       <c r="L16" s="8">
         <f>PAU!D16</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" s="8" t="str">
         <f>PAU!E16</f>
@@ -4843,7 +4843,7 @@
       </c>
       <c r="L17" s="8">
         <f>PAU!D17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" s="8" t="str">
         <f>PAU!E17</f>
@@ -5025,7 +5025,7 @@
       </c>
       <c r="L18" s="8">
         <f>PAU!D18</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="8" t="str">
         <f>PAU!E18</f>
@@ -5207,7 +5207,7 @@
       </c>
       <c r="L19" s="8">
         <f>PAU!D19</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" s="8" t="str">
         <f>PAU!E19</f>
@@ -5389,7 +5389,7 @@
       </c>
       <c r="L20" s="8">
         <f>PAU!D20</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20" s="8" t="str">
         <f>PAU!E20</f>
@@ -5571,7 +5571,7 @@
       </c>
       <c r="L21" s="8">
         <f>PAU!D21</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21" s="8" t="str">
         <f>PAU!E21</f>
@@ -5753,7 +5753,7 @@
       </c>
       <c r="L22" s="8">
         <f>PAU!D22</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" s="8" t="str">
         <f>PAU!E22</f>
@@ -5935,7 +5935,7 @@
       </c>
       <c r="L23" s="8">
         <f>PAU!D23</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" s="8" t="str">
         <f>PAU!E23</f>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="L24" s="8">
         <f>PAU!D24</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" s="8" t="str">
         <f>PAU!E24</f>
@@ -6299,7 +6299,7 @@
       </c>
       <c r="L25" s="8">
         <f>PAU!D25</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" s="8" t="str">
         <f>PAU!E25</f>
@@ -6481,7 +6481,7 @@
       </c>
       <c r="L26" s="8">
         <f>PAU!D26</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" s="8" t="str">
         <f>PAU!E26</f>
@@ -6663,7 +6663,7 @@
       </c>
       <c r="L27" s="8">
         <f>PAU!D27</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="8" t="str">
         <f>PAU!E27</f>
@@ -6845,7 +6845,7 @@
       </c>
       <c r="L28" s="8">
         <f>PAU!D28</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28" s="8" t="str">
         <f>PAU!E28</f>
@@ -7027,7 +7027,7 @@
       </c>
       <c r="L29" s="8">
         <f>PAU!D29</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29" s="8" t="str">
         <f>PAU!E29</f>
@@ -7209,7 +7209,7 @@
       </c>
       <c r="L30" s="8">
         <f>PAU!D30</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30" s="8" t="str">
         <f>PAU!E30</f>
@@ -7391,7 +7391,7 @@
       </c>
       <c r="L31" s="8">
         <f>PAU!D31</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31" s="8" t="str">
         <f>PAU!E31</f>
@@ -7573,7 +7573,7 @@
       </c>
       <c r="L32" s="8">
         <f>PAU!D32</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" s="8" t="str">
         <f>PAU!E32</f>
@@ -7755,7 +7755,7 @@
       </c>
       <c r="L33" s="8">
         <f>PAU!D33</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33" s="8" t="str">
         <f>PAU!E33</f>
@@ -7937,7 +7937,7 @@
       </c>
       <c r="L34" s="8">
         <f>PAU!D34</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34" s="8" t="str">
         <f>PAU!E34</f>
@@ -8119,7 +8119,7 @@
       </c>
       <c r="L35" s="8">
         <f>PAU!D35</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M35" s="8" t="str">
         <f>PAU!E35</f>
@@ -28311,8 +28311,8 @@
   </sheetPr>
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -28390,7 +28390,7 @@
         <v>215</v>
       </c>
       <c r="D3" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>216</v>
@@ -28416,7 +28416,7 @@
         <v>215</v>
       </c>
       <c r="D4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="19" t="s">
         <v>216</v>
@@ -28468,7 +28468,7 @@
         <v>215</v>
       </c>
       <c r="D6" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>216</v>
@@ -28494,7 +28494,7 @@
         <v>215</v>
       </c>
       <c r="D7" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>216</v>
@@ -28520,7 +28520,7 @@
         <v>215</v>
       </c>
       <c r="D8" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>216</v>
@@ -28546,7 +28546,7 @@
         <v>215</v>
       </c>
       <c r="D9" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>216</v>
@@ -28572,7 +28572,7 @@
         <v>215</v>
       </c>
       <c r="D10" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>216</v>
@@ -28598,7 +28598,7 @@
         <v>215</v>
       </c>
       <c r="D11" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>216</v>
@@ -28624,7 +28624,7 @@
         <v>215</v>
       </c>
       <c r="D12" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>216</v>
@@ -28650,7 +28650,7 @@
         <v>215</v>
       </c>
       <c r="D13" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>216</v>
@@ -28676,7 +28676,7 @@
         <v>215</v>
       </c>
       <c r="D14" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>216</v>
@@ -28702,7 +28702,7 @@
         <v>215</v>
       </c>
       <c r="D15" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>216</v>
@@ -28728,7 +28728,7 @@
         <v>215</v>
       </c>
       <c r="D16" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>216</v>
@@ -28754,7 +28754,7 @@
         <v>215</v>
       </c>
       <c r="D17" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>216</v>
@@ -28780,7 +28780,7 @@
         <v>215</v>
       </c>
       <c r="D18" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>216</v>
@@ -28806,7 +28806,7 @@
         <v>215</v>
       </c>
       <c r="D19" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>216</v>
@@ -28832,7 +28832,7 @@
         <v>215</v>
       </c>
       <c r="D20" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>216</v>
@@ -28858,7 +28858,7 @@
         <v>215</v>
       </c>
       <c r="D21" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>216</v>
@@ -28884,7 +28884,7 @@
         <v>215</v>
       </c>
       <c r="D22" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>216</v>
@@ -28910,7 +28910,7 @@
         <v>215</v>
       </c>
       <c r="D23" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>216</v>
@@ -28936,7 +28936,7 @@
         <v>215</v>
       </c>
       <c r="D24" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>216</v>
@@ -28962,7 +28962,7 @@
         <v>215</v>
       </c>
       <c r="D25" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>216</v>
@@ -28988,7 +28988,7 @@
         <v>215</v>
       </c>
       <c r="D26" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>216</v>
@@ -29014,7 +29014,7 @@
         <v>215</v>
       </c>
       <c r="D27" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="19" t="s">
         <v>216</v>
@@ -29040,7 +29040,7 @@
         <v>215</v>
       </c>
       <c r="D28" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="19" t="s">
         <v>216</v>
@@ -29066,7 +29066,7 @@
         <v>215</v>
       </c>
       <c r="D29" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" s="19" t="s">
         <v>216</v>
@@ -29092,7 +29092,7 @@
         <v>215</v>
       </c>
       <c r="D30" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="19" t="s">
         <v>216</v>
@@ -29118,7 +29118,7 @@
         <v>215</v>
       </c>
       <c r="D31" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31" s="19" t="s">
         <v>216</v>
@@ -29144,7 +29144,7 @@
         <v>215</v>
       </c>
       <c r="D32" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>216</v>
@@ -29170,7 +29170,7 @@
         <v>215</v>
       </c>
       <c r="D33" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>216</v>
@@ -29196,7 +29196,7 @@
         <v>215</v>
       </c>
       <c r="D34" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>216</v>
@@ -29222,7 +29222,7 @@
         <v>215</v>
       </c>
       <c r="D35" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>216</v>
@@ -42644,7 +42644,7 @@
   </sheetPr>
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+    <sheetView zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -45795,7 +45795,7 @@
   <dimension ref="A1:AS18"/>
   <sheetViews>
     <sheetView zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="AJ13" sqref="AJ13"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -46009,10 +46009,10 @@
         <v>214</v>
       </c>
       <c r="K2" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="s">
         <v>216</v>

</xml_diff>

<commit_message>
code cleanup and commenting
</commit_message>
<xml_diff>
--- a/HW3/autogen/CUSignals.xlsx
+++ b/HW3/autogen/CUSignals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garre\Desktop\EE 188\HW3\autogen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A2BCB2-7FBC-49CE-8316-E703C5C2553D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDFEE9C-C4D0-4959-BDE5-5212896ED010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-3945" windowWidth="24495" windowHeight="15675" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5592" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5594" uniqueCount="360">
   <si>
     <t>Instruction</t>
   </si>
@@ -1135,9 +1135,6 @@
     <t>BranchSel_BFS</t>
   </si>
   <si>
-    <t>BranchSel_Always</t>
-  </si>
-  <si>
     <t>PAU_Offset8</t>
   </si>
   <si>
@@ -1150,7 +1147,13 @@
     <t>BranchSel_RET</t>
   </si>
   <si>
-    <t>BranchSel_JUMP</t>
+    <t>UseWB</t>
+  </si>
+  <si>
+    <t>BranchSel_Direct</t>
+  </si>
+  <si>
+    <t>BranchSel_Indirect</t>
   </si>
 </sst>
 </file>
@@ -1656,9 +1659,9 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table7" displayName="Table7" ref="A1:I125" totalsRowShown="0">
-  <autoFilter ref="A1:I125" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table7" displayName="Table7" ref="A1:J125" totalsRowShown="0">
+  <autoFilter ref="A1:J125" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Instruction"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="NextState"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="UpdateIR"/>
@@ -1668,6 +1671,7 @@
     <tableColumn id="8" xr3:uid="{4B77E926-C156-4D39-8F23-C4453A726B52}" name="UpdateTempReg2"/>
     <tableColumn id="7" xr3:uid="{4F5AE407-7225-43E3-8C1D-4D80A945FCB4}" name="TempReg2Sel"/>
     <tableColumn id="9" xr3:uid="{4071D217-4E1B-473B-8F81-A216DAD5646F}" name="BranchSel"/>
+    <tableColumn id="10" xr3:uid="{F9A4569D-949C-41DF-971B-D4B8928083B8}" name="UseWB"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1906,11 +1910,11 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AT126"/>
+  <dimension ref="A1:AU126"/>
   <sheetViews>
-    <sheetView zoomScale="69" zoomScaleNormal="103" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AT124" sqref="AT124"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AK1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AU127" sqref="AU127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1956,7 +1960,7 @@
     <col min="46" max="46" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2095,8 +2099,11 @@
       <c r="AT1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="2" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="str">
         <f>ALU!A2</f>
         <v>OpMOV_Imm_To_Rn</v>
@@ -2281,8 +2288,12 @@
         <f>CU!I2</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="3" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU2" s="8">
+        <f>CU!J2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="str">
         <f>ALU!A3</f>
         <v>OpMOVW_At_Disp_PC_To_Rn</v>
@@ -2467,8 +2478,12 @@
         <f>CU!I3</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="4" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU3" s="8">
+        <f>CU!J3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="str">
         <f>ALU!A4</f>
         <v>OpMOVL_At_Disp_PC_To_Rn</v>
@@ -2653,8 +2668,12 @@
         <f>CU!I4</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="5" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU4" s="8">
+        <f>CU!J4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="str">
         <f>ALU!A5</f>
         <v>OpMOV_Rm_To_Rn</v>
@@ -2839,8 +2858,12 @@
         <f>CU!I5</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="6" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU5" s="8">
+        <f>CU!J5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>ALU!A6</f>
         <v>OpMOVB_Rm_To_At_Rn</v>
@@ -3025,8 +3048,12 @@
         <f>CU!I6</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="7" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU6" s="8">
+        <f>CU!J6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>ALU!A7</f>
         <v>OpMOVW_Rm_To_At_Rn</v>
@@ -3211,8 +3238,12 @@
         <f>CU!I7</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="8" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU7" s="8">
+        <f>CU!J7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>ALU!A8</f>
         <v>OpMOVL_Rm_To_At_Rn</v>
@@ -3397,8 +3428,12 @@
         <f>CU!I8</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="9" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU8" s="8">
+        <f>CU!J8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="str">
         <f>ALU!A9</f>
         <v>OpMOVB_At_Rm_To_Rn</v>
@@ -3583,8 +3618,12 @@
         <f>CU!I9</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="10" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU9" s="8">
+        <f>CU!J9</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="str">
         <f>ALU!A10</f>
         <v>OpMOVW_At_Rm_To_Rn</v>
@@ -3769,8 +3808,12 @@
         <f>CU!I10</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="11" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU10" s="8">
+        <f>CU!J10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="str">
         <f>ALU!A11</f>
         <v>OpMOVL_At_Rm_Rn</v>
@@ -3955,8 +3998,12 @@
         <f>CU!I11</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="12" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU11" s="8">
+        <f>CU!J11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="str">
         <f>ALU!A12</f>
         <v>OpMOVB_Rm_To_At_Dec_Rn</v>
@@ -4141,8 +4188,12 @@
         <f>CU!I12</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="13" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU12" s="8">
+        <f>CU!J12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="str">
         <f>ALU!A13</f>
         <v>OpMOVW_Rm_To_At_Dec_Rn</v>
@@ -4327,8 +4378,12 @@
         <f>CU!I13</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="14" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU13" s="8">
+        <f>CU!J13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="str">
         <f>ALU!A14</f>
         <v>OpMOVL_Rm_To_At_Dec_Rn</v>
@@ -4513,8 +4568,12 @@
         <f>CU!I14</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="15" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU14" s="8">
+        <f>CU!J14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="str">
         <f>ALU!A15</f>
         <v>OpMOVB_At_Rm_Inc_To_Rn</v>
@@ -4699,8 +4758,12 @@
         <f>CU!I15</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="16" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU15" s="8">
+        <f>CU!J15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="str">
         <f>ALU!A16</f>
         <v>OpMOVW_At_Rm_Inc_To_Rn</v>
@@ -4885,8 +4948,12 @@
         <f>CU!I16</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="17" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU16" s="8">
+        <f>CU!J16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="str">
         <f>ALU!A17</f>
         <v>OpMOVL_At_Rm_Inc_To_Rn</v>
@@ -5071,8 +5138,12 @@
         <f>CU!I17</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="18" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU17" s="8">
+        <f>CU!J17</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="str">
         <f>ALU!A18</f>
         <v>OpMOVB_R0_To_At_Disp_Rn</v>
@@ -5257,8 +5328,12 @@
         <f>CU!I18</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="19" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU18" s="8">
+        <f>CU!J18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="str">
         <f>ALU!A19</f>
         <v>OpMOVW_R0_To_At_Disp_Rn</v>
@@ -5443,8 +5518,12 @@
         <f>CU!I19</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="20" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU19" s="8">
+        <f>CU!J19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="str">
         <f>ALU!A20</f>
         <v>OpMOVL_R0_To_At_Disp_Rn</v>
@@ -5629,8 +5708,12 @@
         <f>CU!I20</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="21" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU20" s="8">
+        <f>CU!J20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="str">
         <f>ALU!A21</f>
         <v>OpMOVB_At_Disp_Rm_To_R0</v>
@@ -5815,8 +5898,12 @@
         <f>CU!I21</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="22" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU21" s="8">
+        <f>CU!J21</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="str">
         <f>ALU!A22</f>
         <v>OpMOVW_At_Disp_Rm_To_R0</v>
@@ -6001,8 +6088,12 @@
         <f>CU!I22</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="23" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU22" s="8">
+        <f>CU!J22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="str">
         <f>ALU!A23</f>
         <v>OpMOVL_At_Disp_Rm_To_Rn</v>
@@ -6187,8 +6278,12 @@
         <f>CU!I23</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="24" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU23" s="8">
+        <f>CU!J23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="str">
         <f>ALU!A24</f>
         <v>OpMOVB_Rm_To_At_R0_Rn</v>
@@ -6373,8 +6468,12 @@
         <f>CU!I24</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="25" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU24" s="8">
+        <f>CU!J24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="str">
         <f>ALU!A25</f>
         <v>OpMOVW_Rm_To_At_R0_Rn</v>
@@ -6559,8 +6658,12 @@
         <f>CU!I25</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="26" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU25" s="8">
+        <f>CU!J25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="str">
         <f>ALU!A26</f>
         <v>OpMOVL_Rm_To_At_R0_Rn</v>
@@ -6745,8 +6848,12 @@
         <f>CU!I26</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="27" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU26" s="8">
+        <f>CU!J26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="str">
         <f>ALU!A27</f>
         <v>OpMOVB_At_R0_Rm_To_Rn</v>
@@ -6931,8 +7038,12 @@
         <f>CU!I27</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="28" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU27" s="8">
+        <f>CU!J27</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="str">
         <f>ALU!A28</f>
         <v>OpMOVW_At_R0_Rm_To_Rn</v>
@@ -7117,8 +7228,12 @@
         <f>CU!I28</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="29" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU28" s="8">
+        <f>CU!J28</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="str">
         <f>ALU!A29</f>
         <v>OpMOVL_At_R0_Rm_To_Rn</v>
@@ -7303,8 +7418,12 @@
         <f>CU!I29</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="30" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU29" s="8">
+        <f>CU!J29</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="str">
         <f>ALU!A30</f>
         <v>OpMOVB_R0_To_At_Disp_GBR</v>
@@ -7489,8 +7608,12 @@
         <f>CU!I30</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="31" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU30" s="8">
+        <f>CU!J30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="str">
         <f>ALU!A31</f>
         <v>OpMOVW_R0_To_At_Disp_GBR</v>
@@ -7675,8 +7798,12 @@
         <f>CU!I31</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="32" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU31" s="8">
+        <f>CU!J31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="str">
         <f>ALU!A32</f>
         <v>OpMOVL_R0_To_At_Disp_GBR</v>
@@ -7861,8 +7988,12 @@
         <f>CU!I32</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="33" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU32" s="8">
+        <f>CU!J32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="str">
         <f>ALU!A33</f>
         <v>OpMOVB_At_Disp_GBR_To_R0</v>
@@ -8047,8 +8178,12 @@
         <f>CU!I33</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="34" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU33" s="8">
+        <f>CU!J33</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="str">
         <f>ALU!A34</f>
         <v>OpMOVW_At_Disp_GBR_To_R0</v>
@@ -8233,8 +8368,12 @@
         <f>CU!I34</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="35" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU34" s="8">
+        <f>CU!J34</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="str">
         <f>ALU!A35</f>
         <v>OpMOVL_At_Disp_GBR_To_R0</v>
@@ -8419,8 +8558,12 @@
         <f>CU!I35</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="36" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU35" s="8">
+        <f>CU!J35</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="str">
         <f>ALU!A36</f>
         <v>OpMOVA</v>
@@ -8605,8 +8748,12 @@
         <f>CU!I36</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="37" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU36" s="8">
+        <f>CU!J36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="str">
         <f>ALU!A37</f>
         <v>OpMOVT</v>
@@ -8791,8 +8938,12 @@
         <f>CU!I37</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="38" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU37" s="8">
+        <f>CU!J37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="str">
         <f>ALU!A38</f>
         <v>OpSwapB</v>
@@ -8977,8 +9128,12 @@
         <f>CU!I38</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="39" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU38" s="8">
+        <f>CU!J38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="str">
         <f>ALU!A39</f>
         <v>OpSwapW</v>
@@ -9163,8 +9318,12 @@
         <f>CU!I39</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="40" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU39" s="8">
+        <f>CU!J39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="str">
         <f>ALU!A40</f>
         <v>OpXTRCT</v>
@@ -9349,8 +9508,12 @@
         <f>CU!I40</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="41" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU40" s="8">
+        <f>CU!J40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="str">
         <f>ALU!A41</f>
         <v>OpADD_Rm_Rn</v>
@@ -9535,8 +9698,12 @@
         <f>CU!I41</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="42" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU41" s="8">
+        <f>CU!J41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="str">
         <f>ALU!A42</f>
         <v>OpADD_Imm_Rn</v>
@@ -9721,8 +9888,12 @@
         <f>CU!I42</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="43" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU42" s="8">
+        <f>CU!J42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="str">
         <f>ALU!A43</f>
         <v>OpADDC</v>
@@ -9907,8 +10078,12 @@
         <f>CU!I43</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="44" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU43" s="8">
+        <f>CU!J43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="str">
         <f>ALU!A44</f>
         <v>OpADDV</v>
@@ -10093,8 +10268,12 @@
         <f>CU!I44</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="45" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU44" s="8">
+        <f>CU!J44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="str">
         <f>ALU!A45</f>
         <v>OpCMP_EQ_Imm</v>
@@ -10279,8 +10458,12 @@
         <f>CU!I45</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="46" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU45" s="8">
+        <f>CU!J45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="str">
         <f>ALU!A46</f>
         <v>OpCMP_EQ_RmRn</v>
@@ -10465,8 +10648,12 @@
         <f>CU!I46</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="47" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU46" s="8">
+        <f>CU!J46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="str">
         <f>ALU!A47</f>
         <v>OpCMP_HS</v>
@@ -10651,8 +10838,12 @@
         <f>CU!I47</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="48" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU47" s="8">
+        <f>CU!J47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="str">
         <f>ALU!A48</f>
         <v>OpCMP_GE</v>
@@ -10837,8 +11028,12 @@
         <f>CU!I48</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="49" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU48" s="8">
+        <f>CU!J48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="str">
         <f>ALU!A49</f>
         <v>OpCMP_HI</v>
@@ -11023,8 +11218,12 @@
         <f>CU!I49</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="50" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU49" s="8">
+        <f>CU!J49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="str">
         <f>ALU!A50</f>
         <v>OpCMP_GT</v>
@@ -11209,8 +11408,12 @@
         <f>CU!I50</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="51" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU50" s="8">
+        <f>CU!J50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="str">
         <f>ALU!A51</f>
         <v>OpCMP_PL</v>
@@ -11395,8 +11598,12 @@
         <f>CU!I51</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="52" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU51" s="8">
+        <f>CU!J51</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="str">
         <f>ALU!A52</f>
         <v>OpCMP_PZ</v>
@@ -11581,8 +11788,12 @@
         <f>CU!I52</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="53" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU52" s="8">
+        <f>CU!J52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="str">
         <f>ALU!A53</f>
         <v>OpCMP_STR</v>
@@ -11767,8 +11978,12 @@
         <f>CU!I53</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="54" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU53" s="8">
+        <f>CU!J53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="str">
         <f>ALU!A54</f>
         <v>OpDT</v>
@@ -11953,8 +12168,12 @@
         <f>CU!I54</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="55" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU54" s="8">
+        <f>CU!J54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="str">
         <f>ALU!A55</f>
         <v>OpEXTS_B</v>
@@ -12139,8 +12358,12 @@
         <f>CU!I55</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="56" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU55" s="8">
+        <f>CU!J55</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="str">
         <f>ALU!A56</f>
         <v>OpEXTS_W</v>
@@ -12325,8 +12548,12 @@
         <f>CU!I56</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="57" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU56" s="8">
+        <f>CU!J56</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="str">
         <f>ALU!A57</f>
         <v>OpEXTU_B</v>
@@ -12511,8 +12738,12 @@
         <f>CU!I57</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="58" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU57" s="8">
+        <f>CU!J57</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="str">
         <f>ALU!A58</f>
         <v>OpEXTU_W</v>
@@ -12697,8 +12928,12 @@
         <f>CU!I58</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="59" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU58" s="8">
+        <f>CU!J58</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="str">
         <f>ALU!A59</f>
         <v>OpNEG</v>
@@ -12883,8 +13118,12 @@
         <f>CU!I59</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="60" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU59" s="8">
+        <f>CU!J59</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="str">
         <f>ALU!A60</f>
         <v>OpNEGC</v>
@@ -13069,8 +13308,12 @@
         <f>CU!I60</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="61" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU60" s="8">
+        <f>CU!J60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="str">
         <f>ALU!A61</f>
         <v>OpSUB</v>
@@ -13255,8 +13498,12 @@
         <f>CU!I61</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="62" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU61" s="8">
+        <f>CU!J61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="str">
         <f>ALU!A62</f>
         <v>OpSUBC</v>
@@ -13441,8 +13688,12 @@
         <f>CU!I62</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="63" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU62" s="8">
+        <f>CU!J62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="str">
         <f>ALU!A63</f>
         <v>OpSUBV</v>
@@ -13627,8 +13878,12 @@
         <f>CU!I63</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="64" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU63" s="8">
+        <f>CU!J63</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="str">
         <f>ALU!A64</f>
         <v>OpAND_Rm_Rn</v>
@@ -13813,8 +14068,12 @@
         <f>CU!I64</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="65" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU64" s="8">
+        <f>CU!J64</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="str">
         <f>ALU!A65</f>
         <v>OpAND_Imm_Rn</v>
@@ -13999,8 +14258,12 @@
         <f>CU!I65</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="66" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU65" s="8">
+        <f>CU!J65</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="str">
         <f>ALU!A66</f>
         <v>OpAND_Imm_B</v>
@@ -14185,8 +14448,12 @@
         <f>CU!I66</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="67" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU66" s="8">
+        <f>CU!J66</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="str">
         <f>ALU!A67</f>
         <v>OpNOT</v>
@@ -14371,8 +14638,12 @@
         <f>CU!I67</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="68" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU67" s="8">
+        <f>CU!J67</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="str">
         <f>ALU!A68</f>
         <v>OpOR_Rm_Rn</v>
@@ -14557,8 +14828,12 @@
         <f>CU!I68</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="69" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU68" s="8">
+        <f>CU!J68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="str">
         <f>ALU!A69</f>
         <v>OpOR_Imm</v>
@@ -14743,8 +15018,12 @@
         <f>CU!I69</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="70" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU69" s="8">
+        <f>CU!J69</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="str">
         <f>ALU!A70</f>
         <v>OpOR_Imm_B</v>
@@ -14929,8 +15208,12 @@
         <f>CU!I70</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="71" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU70" s="8">
+        <f>CU!J70</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="str">
         <f>ALU!A71</f>
         <v>OpTAS_B</v>
@@ -15115,8 +15398,12 @@
         <f>CU!I71</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="72" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU71" s="8">
+        <f>CU!J71</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="str">
         <f>ALU!A72</f>
         <v>OpTST_Rm_Rn</v>
@@ -15301,8 +15588,12 @@
         <f>CU!I72</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="73" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU72" s="8">
+        <f>CU!J72</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="str">
         <f>ALU!A73</f>
         <v>OpTST_Imm</v>
@@ -15487,8 +15778,12 @@
         <f>CU!I73</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="74" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU73" s="8">
+        <f>CU!J73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="str">
         <f>ALU!A74</f>
         <v>OpTST_Imm_B</v>
@@ -15673,8 +15968,12 @@
         <f>CU!I74</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="75" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU74" s="8">
+        <f>CU!J74</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="str">
         <f>ALU!A75</f>
         <v>OpXOR_Rm_Rn</v>
@@ -15859,8 +16158,12 @@
         <f>CU!I75</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="76" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU75" s="8">
+        <f>CU!J75</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="str">
         <f>ALU!A76</f>
         <v>OpXOR_Imm</v>
@@ -16045,8 +16348,12 @@
         <f>CU!I76</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="77" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU76" s="8">
+        <f>CU!J76</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="str">
         <f>ALU!A77</f>
         <v>OpXOR_Imm_B</v>
@@ -16231,8 +16538,12 @@
         <f>CU!I77</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="78" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU77" s="8">
+        <f>CU!J77</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="str">
         <f>ALU!A78</f>
         <v>OpROTL</v>
@@ -16417,8 +16728,12 @@
         <f>CU!I78</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="79" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU78" s="8">
+        <f>CU!J78</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="str">
         <f>ALU!A79</f>
         <v>OpROTR</v>
@@ -16603,8 +16918,12 @@
         <f>CU!I79</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="80" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU79" s="8">
+        <f>CU!J79</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="str">
         <f>ALU!A80</f>
         <v>OpROTCL</v>
@@ -16789,8 +17108,12 @@
         <f>CU!I80</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="81" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU80" s="8">
+        <f>CU!J80</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="str">
         <f>ALU!A81</f>
         <v>OpROTCR</v>
@@ -16975,8 +17298,12 @@
         <f>CU!I81</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="82" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU81" s="8">
+        <f>CU!J81</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="str">
         <f>ALU!A82</f>
         <v>OpSHAL</v>
@@ -17161,8 +17488,12 @@
         <f>CU!I82</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="83" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU82" s="8">
+        <f>CU!J82</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="str">
         <f>ALU!A83</f>
         <v>OpSHAR</v>
@@ -17347,8 +17678,12 @@
         <f>CU!I83</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="84" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU83" s="8">
+        <f>CU!J83</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="str">
         <f>ALU!A84</f>
         <v>OpSHLL</v>
@@ -17533,8 +17868,12 @@
         <f>CU!I84</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="85" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU84" s="8">
+        <f>CU!J84</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="str">
         <f>ALU!A85</f>
         <v>OpSHLR</v>
@@ -17719,8 +18058,12 @@
         <f>CU!I85</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="86" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU85" s="8">
+        <f>CU!J85</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="str">
         <f>ALU!A86</f>
         <v>OpSHLL2</v>
@@ -17905,8 +18248,12 @@
         <f>CU!I86</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="87" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU86" s="8">
+        <f>CU!J86</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="str">
         <f>ALU!A87</f>
         <v>OpSHLR2</v>
@@ -18091,8 +18438,12 @@
         <f>CU!I87</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="88" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU87" s="8">
+        <f>CU!J87</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="str">
         <f>ALU!A88</f>
         <v>OpSHLL8</v>
@@ -18277,8 +18628,12 @@
         <f>CU!I88</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="89" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU88" s="8">
+        <f>CU!J88</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="str">
         <f>ALU!A89</f>
         <v>OpSHLR8</v>
@@ -18463,8 +18818,12 @@
         <f>CU!I89</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="90" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU89" s="8">
+        <f>CU!J89</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="str">
         <f>ALU!A90</f>
         <v>OpSHLL16</v>
@@ -18649,8 +19008,12 @@
         <f>CU!I90</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="91" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU90" s="8">
+        <f>CU!J90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="str">
         <f>ALU!A91</f>
         <v>OpSHLR16</v>
@@ -18835,8 +19198,12 @@
         <f>CU!I91</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="92" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU91" s="8">
+        <f>CU!J91</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="str">
         <f>ALU!A92</f>
         <v>OpBF</v>
@@ -19021,8 +19388,12 @@
         <f>CU!I92</f>
         <v>BranchSel_BF</v>
       </c>
-    </row>
-    <row r="93" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU92" s="8">
+        <f>CU!J92</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="str">
         <f>ALU!A93</f>
         <v>OpBFS</v>
@@ -19207,8 +19578,12 @@
         <f>CU!I93</f>
         <v>BranchSel_BFS</v>
       </c>
-    </row>
-    <row r="94" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU93" s="8">
+        <f>CU!J93</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="str">
         <f>ALU!A94</f>
         <v>OpBT</v>
@@ -19393,8 +19768,12 @@
         <f>CU!I94</f>
         <v>BranchSel_BT</v>
       </c>
-    </row>
-    <row r="95" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU94" s="8">
+        <f>CU!J94</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="str">
         <f>ALU!A95</f>
         <v>OpBTS</v>
@@ -19579,8 +19958,12 @@
         <f>CU!I95</f>
         <v>BranchSel_BTS</v>
       </c>
-    </row>
-    <row r="96" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU95" s="8">
+        <f>CU!J95</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="str">
         <f>ALU!A96</f>
         <v>OpBRA</v>
@@ -19763,10 +20146,14 @@
       </c>
       <c r="AT96" s="8" t="str">
         <f>CU!I96</f>
-        <v>BranchSel_Always</v>
-      </c>
-    </row>
-    <row r="97" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>BranchSel_Direct</v>
+      </c>
+      <c r="AU96" s="8">
+        <f>CU!J96</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="str">
         <f>ALU!A97</f>
         <v>OpBRAF</v>
@@ -19949,10 +20336,14 @@
       </c>
       <c r="AT97" s="8" t="str">
         <f>CU!I97</f>
-        <v>BranchSel_Always</v>
-      </c>
-    </row>
-    <row r="98" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>BranchSel_Direct</v>
+      </c>
+      <c r="AU97" s="8">
+        <f>CU!J97</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="str">
         <f>ALU!A98</f>
         <v>OpBSR</v>
@@ -20135,10 +20526,14 @@
       </c>
       <c r="AT98" s="8" t="str">
         <f>CU!I98</f>
-        <v>BranchSel_Always</v>
-      </c>
-    </row>
-    <row r="99" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>BranchSel_Direct</v>
+      </c>
+      <c r="AU98" s="8">
+        <f>CU!J98</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="str">
         <f>ALU!A99</f>
         <v>OpBSRF</v>
@@ -20321,10 +20716,14 @@
       </c>
       <c r="AT99" s="8" t="str">
         <f>CU!I99</f>
-        <v>BranchSel_Always</v>
-      </c>
-    </row>
-    <row r="100" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>BranchSel_Direct</v>
+      </c>
+      <c r="AU99" s="8">
+        <f>CU!J99</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="str">
         <f>ALU!A100</f>
         <v>OpJMP</v>
@@ -20507,10 +20906,14 @@
       </c>
       <c r="AT100" s="8" t="str">
         <f>CU!I100</f>
-        <v>BranchSel_JUMP</v>
-      </c>
-    </row>
-    <row r="101" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>BranchSel_Indirect</v>
+      </c>
+      <c r="AU100" s="8">
+        <f>CU!J100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="str">
         <f>ALU!A101</f>
         <v>OpJSR</v>
@@ -20693,10 +21096,14 @@
       </c>
       <c r="AT101" s="8" t="str">
         <f>CU!I101</f>
-        <v>BranchSel_JUMP</v>
-      </c>
-    </row>
-    <row r="102" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>BranchSel_Indirect</v>
+      </c>
+      <c r="AU101" s="8">
+        <f>CU!J101</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="str">
         <f>ALU!A102</f>
         <v>OpRTS</v>
@@ -20881,8 +21288,12 @@
         <f>CU!I102</f>
         <v>BranchSel_RET</v>
       </c>
-    </row>
-    <row r="103" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU102" s="8">
+        <f>CU!J102</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="str">
         <f>ALU!A103</f>
         <v>OpCLRT</v>
@@ -21067,8 +21478,12 @@
         <f>CU!I103</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="104" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU103" s="8">
+        <f>CU!J103</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="str">
         <f>ALU!A104</f>
         <v>OpLDC_Rm_To_SR</v>
@@ -21253,8 +21668,12 @@
         <f>CU!I104</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="105" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU104" s="8">
+        <f>CU!J104</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="str">
         <f>ALU!A105</f>
         <v>OpLDC_Rm_To_GBR</v>
@@ -21439,8 +21858,12 @@
         <f>CU!I105</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="106" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU105" s="8">
+        <f>CU!J105</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="str">
         <f>ALU!A106</f>
         <v>OpLDC_Rm_To_VBR</v>
@@ -21625,8 +22048,12 @@
         <f>CU!I106</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="107" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU106" s="8">
+        <f>CU!J106</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="str">
         <f>ALU!A107</f>
         <v>OpLDCL_At_Rm_Inc_To_SR</v>
@@ -21811,8 +22238,12 @@
         <f>CU!I107</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="108" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU107" s="8">
+        <f>CU!J107</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="str">
         <f>ALU!A108</f>
         <v>OpLDCL_At_Rm_Inc_To_GBR</v>
@@ -21997,8 +22428,12 @@
         <f>CU!I108</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="109" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU108" s="8">
+        <f>CU!J108</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="str">
         <f>ALU!A109</f>
         <v>OpLDCL_At_Rm_Inc_To_VBR</v>
@@ -22183,8 +22618,12 @@
         <f>CU!I109</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="110" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU109" s="8">
+        <f>CU!J109</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="str">
         <f>ALU!A110</f>
         <v>OpLDS_Rm_To_PR</v>
@@ -22369,8 +22808,12 @@
         <f>CU!I110</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="111" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU110" s="8">
+        <f>CU!J110</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="str">
         <f>ALU!A111</f>
         <v>OpLDSL_At_Rm_Inc_To_PR</v>
@@ -22555,8 +22998,12 @@
         <f>CU!I111</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="112" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU111" s="8">
+        <f>CU!J111</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="str">
         <f>ALU!A112</f>
         <v>OpSLEEP</v>
@@ -22741,8 +23188,12 @@
         <f>CU!I112</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="113" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU112" s="8">
+        <f>CU!J112</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="str">
         <f>ALU!A113</f>
         <v>OpNOP</v>
@@ -22927,8 +23378,12 @@
         <f>CU!I113</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="114" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU113" s="8">
+        <f>CU!J113</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="str">
         <f>ALU!A114</f>
         <v>OpRTE</v>
@@ -23113,8 +23568,12 @@
         <f>CU!I114</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU114" s="8">
+        <f>CU!J114</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="str">
         <f>ALU!A115</f>
         <v>OpSETT</v>
@@ -23299,8 +23758,12 @@
         <f>CU!I115</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="116" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU115" s="8">
+        <f>CU!J115</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="str">
         <f>ALU!A116</f>
         <v>OpSTC_SR_To_Rn</v>
@@ -23485,8 +23948,12 @@
         <f>CU!I116</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="117" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU116" s="8">
+        <f>CU!J116</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="str">
         <f>ALU!A117</f>
         <v>OpSTC_GBR_To_Rn</v>
@@ -23671,8 +24138,12 @@
         <f>CU!I117</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="118" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU117" s="8">
+        <f>CU!J117</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="str">
         <f>ALU!A118</f>
         <v>OpSTC_VBR_To_Rn</v>
@@ -23857,8 +24328,12 @@
         <f>CU!I118</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="119" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU118" s="8">
+        <f>CU!J118</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="str">
         <f>ALU!A119</f>
         <v>OpSTCL_SR_To_At_Dec_Rn</v>
@@ -24043,8 +24518,12 @@
         <f>CU!I119</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="120" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU119" s="8">
+        <f>CU!J119</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="str">
         <f>ALU!A120</f>
         <v>OpSTCL_GBR_To_At_Dec_Rn</v>
@@ -24229,8 +24708,12 @@
         <f>CU!I120</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="121" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU120" s="8">
+        <f>CU!J120</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="str">
         <f>ALU!A121</f>
         <v>OpSTCL_VBR_To_At_Dec_Rn</v>
@@ -24415,8 +24898,12 @@
         <f>CU!I121</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="122" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU121" s="8">
+        <f>CU!J121</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="str">
         <f>ALU!A122</f>
         <v>OpSTS_PR_To_Rn</v>
@@ -24601,8 +25088,12 @@
         <f>CU!I122</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="123" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU122" s="8">
+        <f>CU!J122</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="str">
         <f>ALU!A123</f>
         <v>OpSTSL_PR_To_At_Dec_Rn</v>
@@ -24787,8 +25278,12 @@
         <f>CU!I123</f>
         <v>BranchSel_None</v>
       </c>
-    </row>
-    <row r="124" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU123" s="8">
+        <f>CU!J123</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="str">
         <f>ALU!A124</f>
         <v>OpTRAPA</v>
@@ -24973,8 +25468,12 @@
         <f>CU!I124</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:46" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU124" s="8">
+        <f>CU!J124</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:47" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
         <v>44</v>
       </c>
@@ -25158,8 +25657,12 @@
         <f>CU!I125</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU125" s="8">
+        <f>CU!J125</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="14"/>
     </row>
   </sheetData>
@@ -28837,7 +29340,7 @@
   </sheetPr>
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+    <sheetView topLeftCell="A90" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
       <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
@@ -31224,10 +31727,10 @@
         <v>179</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D92" s="8">
         <v>1</v>
@@ -31250,10 +31753,10 @@
         <v>180</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D93" s="8">
         <v>1</v>
@@ -31276,10 +31779,10 @@
         <v>181</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D94" s="8">
         <v>1</v>
@@ -31302,10 +31805,10 @@
         <v>182</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D95" s="8">
         <v>1</v>
@@ -31328,10 +31831,10 @@
         <v>183</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D96" s="8">
         <v>1</v>
@@ -31354,10 +31857,10 @@
         <v>184</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D97" s="8">
         <v>1</v>
@@ -31380,10 +31883,10 @@
         <v>185</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D98" s="8">
         <v>1</v>
@@ -31406,10 +31909,10 @@
         <v>186</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D99" s="8">
         <v>1</v>
@@ -31435,7 +31938,7 @@
         <v>331</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D100" s="8">
         <v>1</v>
@@ -31461,7 +31964,7 @@
         <v>331</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D101" s="8">
         <v>1</v>
@@ -32119,7 +32622,7 @@
   </sheetPr>
   <dimension ref="A1:H125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -43168,10 +43671,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I125"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
+      <selection activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -43184,9 +43687,10 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -43214,8 +43718,11 @@
       <c r="I1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>46</v>
       </c>
@@ -43243,8 +43750,11 @@
       <c r="I2" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>52</v>
       </c>
@@ -43272,8 +43782,11 @@
       <c r="I3" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>56</v>
       </c>
@@ -43301,8 +43814,11 @@
       <c r="I4" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>57</v>
       </c>
@@ -43330,8 +43846,11 @@
       <c r="I5" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>60</v>
       </c>
@@ -43359,8 +43878,11 @@
       <c r="I6" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>61</v>
       </c>
@@ -43388,8 +43910,11 @@
       <c r="I7" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>62</v>
       </c>
@@ -43417,8 +43942,11 @@
       <c r="I8" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>63</v>
       </c>
@@ -43446,8 +43974,11 @@
       <c r="I9" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>64</v>
       </c>
@@ -43475,8 +44006,11 @@
       <c r="I10" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>246</v>
       </c>
@@ -43504,8 +44038,11 @@
       <c r="I11" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>66</v>
       </c>
@@ -43533,8 +44070,11 @@
       <c r="I12" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>67</v>
       </c>
@@ -43562,8 +44102,11 @@
       <c r="I13" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>68</v>
       </c>
@@ -43591,8 +44134,11 @@
       <c r="I14" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>69</v>
       </c>
@@ -43620,8 +44166,11 @@
       <c r="I15" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
@@ -43649,8 +44198,11 @@
       <c r="I16" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>71</v>
       </c>
@@ -43678,8 +44230,11 @@
       <c r="I17" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>72</v>
       </c>
@@ -43707,8 +44262,11 @@
       <c r="I18" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>73</v>
       </c>
@@ -43736,8 +44294,11 @@
       <c r="I19" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>74</v>
       </c>
@@ -43765,8 +44326,11 @@
       <c r="I20" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>75</v>
       </c>
@@ -43794,8 +44358,11 @@
       <c r="I21" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>76</v>
       </c>
@@ -43823,8 +44390,11 @@
       <c r="I22" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>77</v>
       </c>
@@ -43852,8 +44422,11 @@
       <c r="I23" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>78</v>
       </c>
@@ -43881,8 +44454,11 @@
       <c r="I24" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>79</v>
       </c>
@@ -43910,8 +44486,11 @@
       <c r="I25" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>80</v>
       </c>
@@ -43939,8 +44518,11 @@
       <c r="I26" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>81</v>
       </c>
@@ -43968,8 +44550,11 @@
       <c r="I27" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>82</v>
       </c>
@@ -43997,8 +44582,11 @@
       <c r="I28" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>83</v>
       </c>
@@ -44026,8 +44614,11 @@
       <c r="I29" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>84</v>
       </c>
@@ -44055,8 +44646,11 @@
       <c r="I30" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>85</v>
       </c>
@@ -44084,8 +44678,11 @@
       <c r="I31" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>86</v>
       </c>
@@ -44113,8 +44710,11 @@
       <c r="I32" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>87</v>
       </c>
@@ -44142,8 +44742,11 @@
       <c r="I33" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>88</v>
       </c>
@@ -44171,8 +44774,11 @@
       <c r="I34" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>89</v>
       </c>
@@ -44200,8 +44806,11 @@
       <c r="I35" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>90</v>
       </c>
@@ -44229,8 +44838,11 @@
       <c r="I36" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>91</v>
       </c>
@@ -44258,8 +44870,11 @@
       <c r="I37" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>93</v>
       </c>
@@ -44287,8 +44902,11 @@
       <c r="I38" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>94</v>
       </c>
@@ -44316,8 +44934,11 @@
       <c r="I39" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>95</v>
       </c>
@@ -44345,8 +44966,11 @@
       <c r="I40" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>96</v>
       </c>
@@ -44374,8 +44998,11 @@
       <c r="I41" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>98</v>
       </c>
@@ -44403,8 +45030,11 @@
       <c r="I42" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>99</v>
       </c>
@@ -44432,8 +45062,11 @@
       <c r="I43" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>102</v>
       </c>
@@ -44461,8 +45094,11 @@
       <c r="I44" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>104</v>
       </c>
@@ -44490,8 +45126,11 @@
       <c r="I45" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>108</v>
       </c>
@@ -44519,8 +45158,11 @@
       <c r="I46" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>109</v>
       </c>
@@ -44548,8 +45190,11 @@
       <c r="I47" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>110</v>
       </c>
@@ -44577,8 +45222,11 @@
       <c r="I48" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>112</v>
       </c>
@@ -44606,8 +45254,11 @@
       <c r="I49" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>114</v>
       </c>
@@ -44635,8 +45286,11 @@
       <c r="I50" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>116</v>
       </c>
@@ -44664,8 +45318,11 @@
       <c r="I51" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>119</v>
       </c>
@@ -44693,8 +45350,11 @@
       <c r="I52" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>121</v>
       </c>
@@ -44722,8 +45382,11 @@
       <c r="I53" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>220</v>
       </c>
@@ -44751,8 +45414,11 @@
       <c r="I54" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>125</v>
       </c>
@@ -44780,8 +45446,11 @@
       <c r="I55" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>126</v>
       </c>
@@ -44809,8 +45478,11 @@
       <c r="I56" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>127</v>
       </c>
@@ -44838,8 +45510,11 @@
       <c r="I57" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>128</v>
       </c>
@@ -44867,8 +45542,11 @@
       <c r="I58" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>129</v>
       </c>
@@ -44896,8 +45574,11 @@
       <c r="I59" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>131</v>
       </c>
@@ -44925,8 +45606,11 @@
       <c r="I60" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>134</v>
       </c>
@@ -44954,8 +45638,11 @@
       <c r="I61" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>135</v>
       </c>
@@ -44983,8 +45670,11 @@
       <c r="I62" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>136</v>
       </c>
@@ -45012,8 +45702,11 @@
       <c r="I63" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>137</v>
       </c>
@@ -45041,8 +45734,11 @@
       <c r="I64" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>139</v>
       </c>
@@ -45070,8 +45766,11 @@
       <c r="I65" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>141</v>
       </c>
@@ -45099,8 +45798,11 @@
       <c r="I66" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>142</v>
       </c>
@@ -45128,8 +45830,11 @@
       <c r="I67" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>143</v>
       </c>
@@ -45157,8 +45862,11 @@
       <c r="I68" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>145</v>
       </c>
@@ -45186,8 +45894,11 @@
       <c r="I69" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
         <v>146</v>
       </c>
@@ -45215,8 +45926,11 @@
       <c r="I70" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>147</v>
       </c>
@@ -45244,8 +45958,11 @@
       <c r="I71" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>150</v>
       </c>
@@ -45273,8 +45990,11 @@
       <c r="I72" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>151</v>
       </c>
@@ -45302,8 +46022,11 @@
       <c r="I73" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
         <v>152</v>
       </c>
@@ -45331,8 +46054,11 @@
       <c r="I74" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>153</v>
       </c>
@@ -45360,8 +46086,11 @@
       <c r="I75" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>155</v>
       </c>
@@ -45389,8 +46118,11 @@
       <c r="I76" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>156</v>
       </c>
@@ -45418,8 +46150,11 @@
       <c r="I77" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>157</v>
       </c>
@@ -45447,8 +46182,11 @@
       <c r="I78" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>160</v>
       </c>
@@ -45476,8 +46214,11 @@
       <c r="I79" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
         <v>162</v>
       </c>
@@ -45505,8 +46246,11 @@
       <c r="I80" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>164</v>
       </c>
@@ -45534,8 +46278,11 @@
       <c r="I81" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>166</v>
       </c>
@@ -45563,8 +46310,11 @@
       <c r="I82" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>168</v>
       </c>
@@ -45592,8 +46342,11 @@
       <c r="I83" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
         <v>170</v>
       </c>
@@ -45621,8 +46374,11 @@
       <c r="I84" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>171</v>
       </c>
@@ -45650,8 +46406,11 @@
       <c r="I85" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>173</v>
       </c>
@@ -45679,8 +46438,11 @@
       <c r="I86" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>174</v>
       </c>
@@ -45708,8 +46470,11 @@
       <c r="I87" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
         <v>175</v>
       </c>
@@ -45737,8 +46502,11 @@
       <c r="I88" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
         <v>176</v>
       </c>
@@ -45766,8 +46534,11 @@
       <c r="I89" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
         <v>177</v>
       </c>
@@ -45795,8 +46566,11 @@
       <c r="I90" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
         <v>178</v>
       </c>
@@ -45824,8 +46598,11 @@
       <c r="I91" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
         <v>179</v>
       </c>
@@ -45853,8 +46630,11 @@
       <c r="I92" s="36" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
         <v>180</v>
       </c>
@@ -45882,8 +46662,11 @@
       <c r="I93" s="36" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
         <v>181</v>
       </c>
@@ -45911,8 +46694,11 @@
       <c r="I94" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
         <v>182</v>
       </c>
@@ -45940,8 +46726,11 @@
       <c r="I95" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
         <v>183</v>
       </c>
@@ -45967,10 +46756,13 @@
         <v>53</v>
       </c>
       <c r="I96" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
         <v>184</v>
       </c>
@@ -45996,10 +46788,13 @@
         <v>53</v>
       </c>
       <c r="I97" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
         <v>185</v>
       </c>
@@ -46025,10 +46820,13 @@
         <v>53</v>
       </c>
       <c r="I98" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
         <v>186</v>
       </c>
@@ -46054,10 +46852,13 @@
         <v>53</v>
       </c>
       <c r="I99" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
         <v>187</v>
       </c>
@@ -46083,10 +46884,13 @@
         <v>53</v>
       </c>
       <c r="I100" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
         <v>188</v>
       </c>
@@ -46112,10 +46916,13 @@
         <v>53</v>
       </c>
       <c r="I101" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
         <v>189</v>
       </c>
@@ -46141,10 +46948,13 @@
         <v>53</v>
       </c>
       <c r="I102" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
         <v>190</v>
       </c>
@@ -46166,8 +46976,11 @@
       <c r="I103" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
         <v>191</v>
       </c>
@@ -46192,8 +47005,11 @@
       <c r="I104" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
         <v>192</v>
       </c>
@@ -46215,8 +47031,11 @@
       <c r="I105" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
         <v>193</v>
       </c>
@@ -46238,8 +47057,11 @@
       <c r="I106" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
         <v>194</v>
       </c>
@@ -46264,8 +47086,11 @@
       <c r="I107" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
         <v>195</v>
       </c>
@@ -46287,8 +47112,11 @@
       <c r="I108" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
         <v>196</v>
       </c>
@@ -46310,8 +47138,11 @@
       <c r="I109" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
         <v>197</v>
       </c>
@@ -46333,8 +47164,11 @@
       <c r="I110" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
         <v>198</v>
       </c>
@@ -46356,8 +47190,11 @@
       <c r="I111" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
         <v>199</v>
       </c>
@@ -46379,8 +47216,11 @@
       <c r="I112" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
         <v>225</v>
       </c>
@@ -46402,8 +47242,11 @@
       <c r="I113" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
         <v>226</v>
       </c>
@@ -46425,8 +47268,11 @@
       <c r="H114" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
         <v>227</v>
       </c>
@@ -46448,8 +47294,11 @@
       <c r="I115" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
         <v>228</v>
       </c>
@@ -46471,8 +47320,11 @@
       <c r="I116" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
         <v>229</v>
       </c>
@@ -46494,8 +47346,11 @@
       <c r="I117" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
         <v>230</v>
       </c>
@@ -46517,8 +47372,11 @@
       <c r="I118" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
         <v>231</v>
       </c>
@@ -46540,8 +47398,11 @@
       <c r="I119" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
         <v>232</v>
       </c>
@@ -46563,8 +47424,11 @@
       <c r="I120" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
         <v>233</v>
       </c>
@@ -46586,8 +47450,11 @@
       <c r="I121" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
         <v>234</v>
       </c>
@@ -46609,8 +47476,11 @@
       <c r="I122" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
         <v>235</v>
       </c>
@@ -46632,8 +47502,11 @@
       <c r="I123" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
         <v>236</v>
       </c>
@@ -46652,8 +47525,11 @@
       <c r="H124" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
         <v>44</v>
       </c>
@@ -46671,6 +47547,9 @@
       </c>
       <c r="H125" t="s">
         <v>53</v>
+      </c>
+      <c r="J125">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>